<commit_message>
High Variance problem has been detected in the classification model. As such more data shall be collected.
</commit_message>
<xml_diff>
--- a/Second Iteration Data/data_gathered_part_first_segmentation_34.xlsx
+++ b/Second Iteration Data/data_gathered_part_first_segmentation_34.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Passion\Machine Learning\Projects\Semantic_Web_Parser\Second Iteration Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Passion\Machine Learning\Projects\Semantic_Web_Parser_Model_Builder\Second Iteration Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7B50BF-08D9-4AA1-8B39-38FA13AC96B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FF8253-3168-44CF-8681-EB5DC2651B1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1740" windowWidth="9600" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="948" yWindow="780" windowWidth="9600" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J8" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="M21" workbookViewId="0">
+      <selection activeCell="Q29" sqref="B2:Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,11 +2014,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="Q30">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>